<commit_message>
filtro al excel con store funciona, falta ver el setear hora y la creacion del json para reemplazar a la variable datosMo
</commit_message>
<xml_diff>
--- a/checklistMaker/src/views/CheckListGlobal.xlsx
+++ b/checklistMaker/src/views/CheckListGlobal.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="163">
   <si>
     <t>Etapa</t>
   </si>
@@ -1389,7 +1389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1397,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:A61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1447,95 +1447,107 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+    <row r="2" spans="1:12">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="B3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="I3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="6"/>
+      <c r="K3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="7" t="s">
+      <c r="K4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="13" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1543,35 +1555,31 @@
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="B5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="10" t="s">
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="13" t="s">
+      <c r="K5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="20" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1579,27 +1587,23 @@
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>5</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F6" s="19"/>
       <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>9</v>
-      </c>
+      <c r="H6" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
       <c r="K6" s="20" t="s">
         <v>10</v>
       </c>
@@ -1612,26 +1616,26 @@
         <v>15</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="17"/>
+        <v>28</v>
+      </c>
+      <c r="D7" s="21"/>
       <c r="E7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="19"/>
+        <v>29</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>5</v>
+      </c>
       <c r="G7" s="19"/>
-      <c r="H7" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="22" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1640,20 +1644,20 @@
         <v>15</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="21"/>
+        <v>31</v>
+      </c>
+      <c r="D8" s="17"/>
       <c r="E8" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>5</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
+      <c r="H8" s="19" t="s">
+        <v>7</v>
+      </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
       <c r="K8" s="20" t="s">
@@ -1668,56 +1672,64 @@
         <v>15</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="17"/>
+        <v>34</v>
+      </c>
+      <c r="D9" s="16"/>
       <c r="E9" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+        <v>35</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>6</v>
+      </c>
       <c r="H9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="I9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1">
       <c r="A10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="19" t="s">
+      <c r="I10" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="32" t="s">
         <v>9</v>
       </c>
       <c r="K10" s="24" t="s">
@@ -1727,67 +1739,65 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1">
+    <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>7</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
       <c r="I11" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="32" t="s">
-        <v>9</v>
-      </c>
+      <c r="J11" s="32"/>
       <c r="K11" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="24" t="s">
-        <v>11</v>
-      </c>
+      <c r="L11" s="24"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="32"/>
+        <v>45</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>5</v>
+      </c>
       <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
+      <c r="H12" s="32" t="s">
+        <v>7</v>
+      </c>
       <c r="I12" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="32"/>
+      <c r="J12" s="32" t="s">
+        <v>9</v>
+      </c>
       <c r="K12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L12" s="24"/>
+      <c r="L12" s="24" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
@@ -1797,25 +1807,19 @@
         <v>43</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D13" s="31"/>
       <c r="E13" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="J13" s="32" t="s">
-        <v>9</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
       <c r="K13" s="24" t="s">
         <v>10</v>
       </c>
@@ -1828,14 +1832,14 @@
         <v>42</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="30" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="32" t="s">
@@ -1855,79 +1859,77 @@
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32" t="s">
+      <c r="B15" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="35"/>
+      <c r="E15" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="H15" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D16" s="35"/>
       <c r="E16" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="J16" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="37" t="s">
-        <v>11</v>
-      </c>
+      <c r="K16" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="39"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="35"/>
+        <v>58</v>
+      </c>
+      <c r="D17" s="34"/>
       <c r="E17" s="34" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F17" s="38"/>
       <c r="G17" s="38"/>
@@ -1941,31 +1943,37 @@
       </c>
       <c r="L17" s="39"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1">
+    <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K18" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="39"/>
+      <c r="K18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" s="20" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="3" t="s">
@@ -1975,23 +1983,19 @@
         <v>60</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>5</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F19" s="19"/>
       <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="J19" s="19" t="s">
-        <v>9</v>
-      </c>
+      <c r="H19" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
       <c r="K19" s="20" t="s">
         <v>10</v>
       </c>
@@ -2004,22 +2008,22 @@
         <v>98</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
-      <c r="H20" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="H20" s="19"/>
       <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
+      <c r="J20" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="K20" s="20" t="s">
         <v>10</v>
       </c>
@@ -2041,13 +2045,15 @@
       <c r="E21" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="19" t="s">
+        <v>5</v>
+      </c>
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19" t="s">
-        <v>9</v>
-      </c>
+      <c r="I21" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="19"/>
       <c r="K21" s="20" t="s">
         <v>10</v>
       </c>
@@ -2060,24 +2066,28 @@
         <v>98</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="16" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>5</v>
       </c>
       <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="H22" s="19" t="s">
+        <v>7</v>
+      </c>
       <c r="I22" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J22" s="19"/>
+      <c r="J22" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="K22" s="20" t="s">
         <v>10</v>
       </c>
@@ -2090,22 +2100,20 @@
         <v>98</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F23" s="19" t="s">
         <v>5</v>
       </c>
       <c r="G23" s="19"/>
-      <c r="H23" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="H23" s="19"/>
       <c r="I23" s="19" t="s">
         <v>8</v>
       </c>
@@ -2124,14 +2132,14 @@
         <v>98</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F24" s="19" t="s">
         <v>5</v>
@@ -2159,23 +2167,19 @@
         <v>73</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>5</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="F25" s="19"/>
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
       <c r="I25" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J25" s="19" t="s">
-        <v>9</v>
-      </c>
+      <c r="J25" s="19"/>
       <c r="K25" s="20" t="s">
         <v>10</v>
       </c>
@@ -2188,14 +2192,14 @@
         <v>98</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -2207,49 +2211,47 @@
       <c r="K26" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L26" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="L26" s="20"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="J27" s="19"/>
-      <c r="K27" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="L27" s="20"/>
+      <c r="B27" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="41"/>
+      <c r="E27" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" s="42"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D28" s="41"/>
       <c r="E28" s="40" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F28" s="42"/>
       <c r="G28" s="42"/>
@@ -2258,7 +2260,9 @@
         <v>8</v>
       </c>
       <c r="J28" s="42"/>
-      <c r="K28" s="20"/>
+      <c r="K28" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="L28" s="20" t="s">
         <v>11</v>
       </c>
@@ -2267,22 +2271,22 @@
       <c r="A29" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>83</v>
+      <c r="B29" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="C29" s="40" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D29" s="41"/>
-      <c r="E29" s="40" t="s">
-        <v>85</v>
+      <c r="E29" s="43" t="s">
+        <v>88</v>
       </c>
       <c r="F29" s="42"/>
       <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42" t="s">
-        <v>8</v>
-      </c>
+      <c r="H29" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="42"/>
       <c r="J29" s="42"/>
       <c r="K29" s="20" t="s">
         <v>10</v>
@@ -2295,15 +2299,15 @@
       <c r="A30" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>86</v>
+      <c r="B30" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="43" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="40" t="s">
+        <v>91</v>
       </c>
       <c r="F30" s="42"/>
       <c r="G30" s="42"/>
@@ -2323,23 +2327,23 @@
       <c r="A31" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
+      <c r="B31" s="44">
+        <v>2114</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
       <c r="H31" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
       <c r="K31" s="20" t="s">
         <v>10</v>
       </c>
@@ -2352,14 +2356,14 @@
         <v>98</v>
       </c>
       <c r="B32" s="44">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D32" s="18"/>
-      <c r="E32" s="16" t="s">
-        <v>93</v>
+      <c r="E32" s="45" t="s">
+        <v>95</v>
       </c>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
@@ -2368,26 +2372,24 @@
       </c>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
-      <c r="K32" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="K32" s="20"/>
       <c r="L32" s="20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" ht="90">
       <c r="A33" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B33" s="44">
-        <v>2113</v>
+        <v>2115</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="45" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
@@ -2396,62 +2398,70 @@
       </c>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="90">
+      <c r="K33" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L33" s="20"/>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="44">
-        <v>2115</v>
+      <c r="B34" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="D34" s="18"/>
-      <c r="E34" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="F34" s="19"/>
+      <c r="E34" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>5</v>
+      </c>
       <c r="G34" s="19"/>
-      <c r="H34" s="42" t="s">
+      <c r="H34" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
+      <c r="I34" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="K34" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L34" s="20"/>
+      <c r="L34" s="20" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F35" s="19" t="s">
+      <c r="B35" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19" t="s">
+      <c r="G35" s="42"/>
+      <c r="H35" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="I35" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="J35" s="19" t="s">
+      <c r="I35" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="42" t="s">
         <v>9</v>
       </c>
       <c r="K35" s="20" t="s">
@@ -2466,28 +2476,22 @@
         <v>98</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D36" s="12"/>
-      <c r="E36" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="F36" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="I36" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="J36" s="42" t="s">
-        <v>9</v>
-      </c>
+      <c r="E36" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
       <c r="K36" s="20" t="s">
         <v>10</v>
       </c>
@@ -2509,13 +2513,19 @@
       <c r="E37" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
+      <c r="F37" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" s="42" t="s">
+        <v>9</v>
+      </c>
       <c r="K37" s="20" t="s">
         <v>10</v>
       </c>
@@ -2523,65 +2533,59 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" ht="15.75" thickBot="1">
       <c r="A38" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="F38" s="42" t="s">
+      <c r="B38" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="26"/>
+      <c r="E38" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="50"/>
+      <c r="E39" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="F39" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="J38" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="K38" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="L38" s="20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A39" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="F39" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28" t="s">
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="51"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2589,29 +2593,31 @@
       <c r="A40" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B40" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="D40" s="50"/>
-      <c r="E40" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="F40" s="51" t="s">
+      <c r="B40" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="52"/>
+      <c r="E40" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="J40" s="51"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="24" t="s">
-        <v>11</v>
-      </c>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K40" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="L40" s="53"/>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="3" t="s">
@@ -2625,19 +2631,15 @@
       </c>
       <c r="D41" s="52"/>
       <c r="E41" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="F41" s="32" t="s">
-        <v>5</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="F41" s="32"/>
       <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="J41" s="32" t="s">
-        <v>9</v>
-      </c>
+      <c r="H41" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
       <c r="K41" s="53" t="s">
         <v>10</v>
       </c>
@@ -2648,26 +2650,32 @@
         <v>121</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D42" s="52"/>
       <c r="E42" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="F42" s="32"/>
+        <v>119</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>5</v>
+      </c>
       <c r="G42" s="32"/>
-      <c r="H42" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J42" s="32" t="s">
+        <v>9</v>
+      </c>
       <c r="K42" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="L42" s="53"/>
+      <c r="L42" s="53" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="3" t="s">
@@ -2680,23 +2688,17 @@
         <v>118</v>
       </c>
       <c r="D43" s="52"/>
-      <c r="E43" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="F43" s="32" t="s">
-        <v>5</v>
-      </c>
+      <c r="E43" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="F43" s="32"/>
       <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="J43" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K43" s="53" t="s">
-        <v>10</v>
-      </c>
+      <c r="H43" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="53"/>
       <c r="L43" s="53" t="s">
         <v>11</v>
       </c>
@@ -2706,23 +2708,27 @@
         <v>121</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D44" s="52"/>
-      <c r="E44" s="54" t="s">
-        <v>120</v>
+      <c r="E44" s="30" t="s">
+        <v>124</v>
       </c>
       <c r="F44" s="32"/>
       <c r="G44" s="32"/>
-      <c r="H44" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="I44" s="32"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="53"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K44" s="53" t="s">
+        <v>10</v>
+      </c>
       <c r="L44" s="53" t="s">
         <v>11</v>
       </c>
@@ -2732,21 +2738,19 @@
         <v>121</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="52"/>
+        <v>126</v>
+      </c>
+      <c r="D45" s="23"/>
       <c r="E45" s="30" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F45" s="32"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
-      <c r="I45" s="32" t="s">
-        <v>8</v>
-      </c>
+      <c r="I45" s="32"/>
       <c r="J45" s="32" t="s">
         <v>9</v>
       </c>
@@ -2761,26 +2765,24 @@
       <c r="A46" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="33" t="s">
         <v>125</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="F46" s="32"/>
+        <v>128</v>
+      </c>
+      <c r="D46" s="52"/>
+      <c r="E46" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>5</v>
+      </c>
       <c r="G46" s="32"/>
       <c r="H46" s="32"/>
       <c r="I46" s="32"/>
-      <c r="J46" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K46" s="53" t="s">
-        <v>10</v>
-      </c>
+      <c r="J46" s="32"/>
+      <c r="K46" s="53"/>
       <c r="L46" s="53" t="s">
         <v>11</v>
       </c>
@@ -2790,24 +2792,24 @@
         <v>121</v>
       </c>
       <c r="B47" s="33" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="D47" s="52"/>
-      <c r="E47" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="F47" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="53"/>
-      <c r="L47" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="50"/>
+      <c r="E47" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47" s="51"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="24" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2816,23 +2818,29 @@
         <v>121</v>
       </c>
       <c r="B48" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
+      </c>
+      <c r="C48" s="49" t="s">
+        <v>134</v>
       </c>
       <c r="D48" s="50"/>
       <c r="E48" s="49" t="s">
-        <v>132</v>
-      </c>
-      <c r="F48" s="51"/>
+        <v>135</v>
+      </c>
+      <c r="F48" s="51" t="s">
+        <v>5</v>
+      </c>
       <c r="G48" s="51"/>
       <c r="H48" s="51"/>
       <c r="I48" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="J48" s="51"/>
-      <c r="K48" s="24"/>
+      <c r="J48" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="K48" s="24" t="s">
+        <v>10</v>
+      </c>
       <c r="L48" s="24" t="s">
         <v>11</v>
       </c>
@@ -2842,30 +2850,24 @@
         <v>121</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="C49" s="49" t="s">
-        <v>134</v>
-      </c>
-      <c r="D49" s="50"/>
-      <c r="E49" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="F49" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="G49" s="51"/>
-      <c r="H49" s="51"/>
-      <c r="I49" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="J49" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="K49" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="L49" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" s="23"/>
+      <c r="E49" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J49" s="32"/>
+      <c r="K49" s="53"/>
+      <c r="L49" s="53" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2874,24 +2876,26 @@
         <v>121</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="D50" s="23"/>
-      <c r="E50" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="J50" s="32"/>
-      <c r="K50" s="53"/>
-      <c r="L50" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" s="50"/>
+      <c r="E50" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="F50" s="51"/>
+      <c r="G50" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="H50" s="51"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="51"/>
+      <c r="K50" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L50" s="20" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2903,23 +2907,29 @@
         <v>139</v>
       </c>
       <c r="C51" s="49" t="s">
-        <v>140</v>
-      </c>
-      <c r="D51" s="50"/>
-      <c r="E51" s="56" t="s">
-        <v>141</v>
-      </c>
-      <c r="F51" s="51"/>
-      <c r="G51" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" s="51"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="51"/>
-      <c r="K51" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="L51" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D51" s="52"/>
+      <c r="E51" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="F51" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="J51" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="K51" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="L51" s="24" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2927,32 +2937,24 @@
       <c r="A52" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B52" s="33" t="s">
-        <v>139</v>
+      <c r="B52" s="57">
+        <v>3145</v>
       </c>
       <c r="C52" s="49" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D52" s="52"/>
       <c r="E52" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="F52" s="51" t="s">
-        <v>5</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="F52" s="51"/>
       <c r="G52" s="51"/>
-      <c r="H52" s="51" t="s">
-        <v>7</v>
-      </c>
+      <c r="H52" s="51"/>
       <c r="I52" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="J52" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="K52" s="24" t="s">
-        <v>10</v>
-      </c>
+      <c r="J52" s="51"/>
+      <c r="K52" s="24"/>
       <c r="L52" s="24" t="s">
         <v>11</v>
       </c>
@@ -2961,187 +2963,187 @@
       <c r="A53" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B53" s="57">
-        <v>3145</v>
-      </c>
-      <c r="C53" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="D53" s="52"/>
-      <c r="E53" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="F53" s="51"/>
-      <c r="G53" s="51"/>
-      <c r="H53" s="51"/>
-      <c r="I53" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="J53" s="51"/>
-      <c r="K53" s="24"/>
-      <c r="L53" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="B53" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="D53" s="60"/>
+      <c r="E53" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J53" s="32"/>
+      <c r="K53" s="53"/>
+      <c r="L53" s="53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="45">
       <c r="A54" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B54" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="C54" s="59" t="s">
-        <v>145</v>
-      </c>
-      <c r="D54" s="60"/>
-      <c r="E54" s="61" t="s">
-        <v>146</v>
-      </c>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
+        <v>147</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" s="23"/>
+      <c r="E54" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G54" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" s="32" t="s">
+        <v>7</v>
+      </c>
       <c r="I54" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="J54" s="32"/>
-      <c r="K54" s="53"/>
+      <c r="J54" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K54" s="53" t="s">
+        <v>10</v>
+      </c>
       <c r="L54" s="53" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="45">
+    <row r="55" spans="1:12">
       <c r="A55" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B55" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="C55" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D55" s="23"/>
-      <c r="E55" s="63" t="s">
-        <v>149</v>
-      </c>
-      <c r="F55" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="G55" s="32" t="s">
-        <v>6</v>
-      </c>
+      <c r="B55" s="62">
+        <v>3175</v>
+      </c>
+      <c r="C55" s="61" t="s">
+        <v>150</v>
+      </c>
+      <c r="D55" s="60"/>
+      <c r="E55" s="61" t="s">
+        <v>151</v>
+      </c>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
       <c r="H55" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I55" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="J55" s="32" t="s">
-        <v>9</v>
-      </c>
+      <c r="I55" s="32"/>
+      <c r="J55" s="32"/>
       <c r="K55" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="L55" s="53" t="s">
-        <v>11</v>
-      </c>
+      <c r="L55" s="53"/>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B56" s="62">
-        <v>3175</v>
+      <c r="B56" s="33" t="s">
+        <v>152</v>
       </c>
       <c r="C56" s="61" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D56" s="60"/>
       <c r="E56" s="61" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F56" s="32"/>
       <c r="G56" s="32"/>
-      <c r="H56" s="32" t="s">
-        <v>7</v>
-      </c>
+      <c r="H56" s="32"/>
       <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
+      <c r="J56" s="32" t="s">
+        <v>9</v>
+      </c>
       <c r="K56" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="L56" s="53"/>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="L56" s="53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="30">
       <c r="A57" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="33" t="s">
-        <v>152</v>
+      <c r="B57" s="62">
+        <v>3181</v>
       </c>
       <c r="C57" s="61" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D57" s="60"/>
-      <c r="E57" s="61" t="s">
-        <v>154</v>
-      </c>
-      <c r="F57" s="32"/>
+      <c r="E57" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>5</v>
+      </c>
       <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K57" s="53" t="s">
-        <v>10</v>
-      </c>
+      <c r="H57" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I57" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J57" s="32"/>
+      <c r="K57" s="53"/>
       <c r="L57" s="53" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="30">
+    <row r="58" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="A58" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B58" s="62">
-        <v>3181</v>
+        <v>3171</v>
       </c>
       <c r="C58" s="61" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D58" s="60"/>
-      <c r="E58" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="F58" s="32" t="s">
-        <v>5</v>
-      </c>
+      <c r="E58" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="F58" s="32"/>
       <c r="G58" s="32"/>
       <c r="H58" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I58" s="32" t="s">
-        <v>8</v>
-      </c>
+      <c r="I58" s="32"/>
       <c r="J58" s="32"/>
-      <c r="K58" s="53"/>
-      <c r="L58" s="53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="K58" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="L58" s="53"/>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B59" s="62">
-        <v>3171</v>
+        <v>3182</v>
       </c>
       <c r="C59" s="61" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D59" s="60"/>
-      <c r="E59" s="65" t="s">
-        <v>158</v>
+      <c r="E59" s="66" t="s">
+        <v>160</v>
       </c>
       <c r="F59" s="32"/>
       <c r="G59" s="32"/>
@@ -3153,67 +3155,41 @@
       <c r="K59" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="L59" s="53"/>
+      <c r="L59" s="53" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B60" s="62">
-        <v>3182</v>
+        <v>3183</v>
       </c>
       <c r="C60" s="61" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D60" s="60"/>
-      <c r="E60" s="66" t="s">
-        <v>160</v>
-      </c>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
+      <c r="E60" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="F60" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G60" s="32" t="s">
+        <v>6</v>
+      </c>
       <c r="H60" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I60" s="32"/>
+      <c r="I60" s="32" t="s">
+        <v>8</v>
+      </c>
       <c r="J60" s="32"/>
       <c r="K60" s="53" t="s">
         <v>10</v>
       </c>
       <c r="L60" s="53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
-      <c r="A61" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B61" s="62">
-        <v>3183</v>
-      </c>
-      <c r="C61" s="61" t="s">
-        <v>161</v>
-      </c>
-      <c r="D61" s="60"/>
-      <c r="E61" s="61" t="s">
-        <v>162</v>
-      </c>
-      <c r="F61" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="G61" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="H61" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="I61" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="J61" s="32"/>
-      <c r="K61" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="L61" s="53" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>